<commit_message>
new RF and DT classification models
</commit_message>
<xml_diff>
--- a/Normative Athlete Data - PCSS & MFQ.xlsx
+++ b/Normative Athlete Data - PCSS & MFQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\思庭\AppData\Local\Programs\Python\Python313\dataverse_files tbi Dec 2024 ML Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F971837-05FB-4946-A5A5-BE22270EC994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B130098-8686-4E69-8676-DFB56BE530E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
   <si>
     <t xml:space="preserve">Participant ID </t>
   </si>
@@ -307,11 +307,20 @@
   <si>
     <t>Avg Difference</t>
   </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Avg MFQ Score</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -341,12 +350,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -629,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BT164"/>
+  <dimension ref="A1:BT172"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="F146" workbookViewId="0">
-      <selection activeCell="I168" sqref="I168"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -34711,15 +34723,15 @@
         <v>Soccer 1</v>
       </c>
       <c r="H159" s="1">
-        <f>COUNTIFS($D$2:$D$156,F159)</f>
+        <f t="shared" ref="H159:H164" si="0">COUNTIFS($D$2:$D$156,F159)</f>
         <v>25</v>
       </c>
       <c r="I159" s="1">
-        <f>COUNTIFS($D$2:$D$156,F159,$C$2:$C$156,1)</f>
+        <f t="shared" ref="I159:I164" si="1">COUNTIFS($D$2:$D$156,F159,$C$2:$C$156,1)</f>
         <v>12</v>
       </c>
       <c r="J159" s="1">
-        <f>COUNTIFS($D$2:$D$156,F159,$C$2:$C$156,0)</f>
+        <f t="shared" ref="J159:J164" si="2">COUNTIFS($D$2:$D$156,F159,$C$2:$C$156,0)</f>
         <v>13</v>
       </c>
       <c r="K159" s="2">
@@ -34754,19 +34766,19 @@
         <v>2</v>
       </c>
       <c r="G160" s="1" t="str">
-        <f t="shared" ref="G160:G164" si="0">E160&amp;" "&amp;F160</f>
+        <f t="shared" ref="G160:G164" si="3">E160&amp;" "&amp;F160</f>
         <v>Hockey 2</v>
       </c>
       <c r="H160" s="1">
-        <f>COUNTIFS($D$2:$D$156,F160)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="I160" s="1">
-        <f>COUNTIFS($D$2:$D$156,F160,$C$2:$C$156,1)</f>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="J160" s="1">
-        <f>COUNTIFS($D$2:$D$156,F160,$C$2:$C$156,0)</f>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="K160" s="2">
@@ -34778,7 +34790,7 @@
         <v>6.774193548387097</v>
       </c>
       <c r="M160" s="2">
-        <f t="shared" ref="M160:M164" si="1">K160-L160</f>
+        <f t="shared" ref="M160:M164" si="4">K160-L160</f>
         <v>-3.6972704714640199</v>
       </c>
     </row>
@@ -34797,19 +34809,19 @@
         <v>3</v>
       </c>
       <c r="G161" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Rugby 3</v>
+      </c>
+      <c r="H161" s="1">
         <f t="shared" si="0"/>
-        <v>Rugby 3</v>
-      </c>
-      <c r="H161" s="1">
-        <f>COUNTIFS($D$2:$D$156,F161)</f>
         <v>18</v>
       </c>
       <c r="I161" s="1">
-        <f>COUNTIFS($D$2:$D$156,F161,$C$2:$C$156,1)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J161" s="1">
-        <f>COUNTIFS($D$2:$D$156,F161,$C$2:$C$156,0)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="K161" s="2">
@@ -34821,7 +34833,7 @@
         <v>17.625</v>
       </c>
       <c r="M161" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-13.125</v>
       </c>
     </row>
@@ -34836,19 +34848,19 @@
         <v>4</v>
       </c>
       <c r="G162" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Football 4</v>
+      </c>
+      <c r="H162" s="1">
         <f t="shared" si="0"/>
-        <v>Football 4</v>
-      </c>
-      <c r="H162" s="1">
-        <f>COUNTIFS($D$2:$D$156,F162)</f>
         <v>0</v>
       </c>
       <c r="I162" s="1">
-        <f>COUNTIFS($D$2:$D$156,F162,$C$2:$C$156,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J162" s="1">
-        <f>COUNTIFS($D$2:$D$156,F162,$C$2:$C$156,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K162" s="2">
@@ -34858,7 +34870,7 @@
         <v>0</v>
       </c>
       <c r="M162" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -34870,19 +34882,19 @@
         <v>5</v>
       </c>
       <c r="G163" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Lacrosse 5</v>
+      </c>
+      <c r="H163" s="1">
         <f t="shared" si="0"/>
-        <v>Lacrosse 5</v>
-      </c>
-      <c r="H163" s="1">
-        <f>COUNTIFS($D$2:$D$156,F163)</f>
         <v>23</v>
       </c>
       <c r="I163" s="1">
-        <f>COUNTIFS($D$2:$D$156,F163,$C$2:$C$156,1)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="J163" s="1">
-        <f>COUNTIFS($D$2:$D$156,F163,$C$2:$C$156,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K163" s="2">
@@ -34893,7 +34905,7 @@
         <v>0</v>
       </c>
       <c r="M163" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.0869565217391304</v>
       </c>
     </row>
@@ -34905,19 +34917,19 @@
         <v>6</v>
       </c>
       <c r="G164" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Cheerleading 6</v>
+      </c>
+      <c r="H164" s="1">
         <f t="shared" si="0"/>
-        <v>Cheerleading 6</v>
-      </c>
-      <c r="H164" s="1">
-        <f>COUNTIFS($D$2:$D$156,F164)</f>
         <v>19</v>
       </c>
       <c r="I164" s="1">
-        <f>COUNTIFS($D$2:$D$156,F164,$C$2:$C$156,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J164" s="1">
-        <f>COUNTIFS($D$2:$D$156,F164,$C$2:$C$156,0)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="K164" s="2">
@@ -34928,8 +34940,64 @@
         <v>19.631578947368421</v>
       </c>
       <c r="M164" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-19.631578947368421</v>
+      </c>
+    </row>
+    <row r="166" spans="3:13" x14ac:dyDescent="0.5">
+      <c r="D166" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="167" spans="3:13" x14ac:dyDescent="0.5">
+      <c r="D167" s="1">
+        <v>13</v>
+      </c>
+      <c r="E167" s="3">
+        <v>4.2926829268292686</v>
+      </c>
+    </row>
+    <row r="168" spans="3:13" x14ac:dyDescent="0.5">
+      <c r="D168" s="1">
+        <v>14</v>
+      </c>
+      <c r="E168" s="3">
+        <v>7.9714285714285715</v>
+      </c>
+    </row>
+    <row r="169" spans="3:13" x14ac:dyDescent="0.5">
+      <c r="D169" s="1">
+        <v>15</v>
+      </c>
+      <c r="E169" s="3">
+        <v>8.875</v>
+      </c>
+    </row>
+    <row r="170" spans="3:13" x14ac:dyDescent="0.5">
+      <c r="D170" s="1">
+        <v>16</v>
+      </c>
+      <c r="E170" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="171" spans="3:13" x14ac:dyDescent="0.5">
+      <c r="D171" s="1">
+        <v>17</v>
+      </c>
+      <c r="E171" s="3">
+        <v>7.9230769230769234</v>
+      </c>
+    </row>
+    <row r="172" spans="3:13" x14ac:dyDescent="0.5">
+      <c r="D172" s="1">
+        <v>18</v>
+      </c>
+      <c r="E172" s="3">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated feature engineering, learning curve analysis, and cleaned data
</commit_message>
<xml_diff>
--- a/Normative Athlete Data - PCSS & MFQ.xlsx
+++ b/Normative Athlete Data - PCSS & MFQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\思庭\AppData\Local\Programs\Python\Python313\dataverse_files tbi Dec 2024 ML Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B130098-8686-4E69-8676-DFB56BE530E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9801EC-B32A-4AE1-BC2B-F3AEAB93AB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
   <si>
     <t xml:space="preserve">Participant ID </t>
   </si>
@@ -313,13 +313,22 @@
   <si>
     <t>Avg MFQ Score</t>
   </si>
+  <si>
+    <t>Manova on the entire dataset</t>
+  </si>
+  <si>
+    <t>between (diff sports) and within(MvF) group test. Mann whiteney for MvF since it's not normally distributed. Kruscal wallace for in between in sports</t>
+  </si>
+  <si>
+    <t>How to bring together what are the differences between groups in the dataset and ranking risk factors. Do risk factors change results even if theyre the same for a man v a woman</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -358,7 +367,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -643,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BT172"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="E167" sqref="E167"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E157" zoomScale="87" workbookViewId="0">
+      <selection activeCell="G169" sqref="G169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -34944,6 +34953,10 @@
         <v>-19.631578947368421</v>
       </c>
     </row>
+    <row r="165" spans="3:13" x14ac:dyDescent="0.5">
+      <c r="I165" s="1"/>
+      <c r="J165" s="1"/>
+    </row>
     <row r="166" spans="3:13" x14ac:dyDescent="0.5">
       <c r="D166" s="1" t="s">
         <v>88</v>
@@ -34967,6 +34980,9 @@
       <c r="E168" s="3">
         <v>7.9714285714285715</v>
       </c>
+      <c r="G168" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="169" spans="3:13" x14ac:dyDescent="0.5">
       <c r="D169" s="1">
@@ -34975,6 +34991,9 @@
       <c r="E169" s="3">
         <v>8.875</v>
       </c>
+      <c r="G169" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="170" spans="3:13" x14ac:dyDescent="0.5">
       <c r="D170" s="1">
@@ -34982,6 +35001,9 @@
       </c>
       <c r="E170" s="3">
         <v>11</v>
+      </c>
+      <c r="G170" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="171" spans="3:13" x14ac:dyDescent="0.5">

</xml_diff>